<commit_message>
few scequences names updated
</commit_message>
<xml_diff>
--- a/SportsInviter/Data/Config.xlsx
+++ b/SportsInviter/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arun\Documents\UiPath\RoboticEnterpriseFrameworkTest\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arun\Documents\UiPath\PUA2019\SportsInviter\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57A4935-C0C2-4903-BE33-95F8D4C1FEA3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDD299E-73D8-49BF-8008-E662F0E341D6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="64">
   <si>
     <t>Name</t>
   </si>
@@ -196,6 +196,24 @@
   </si>
   <si>
     <t>strWeatherAPIEndpoint</t>
+  </si>
+  <si>
+    <t>API key from Open weather map</t>
+  </si>
+  <si>
+    <t>Google API Key for accessing location and calendar cloud apps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Google Client ID for accessing Calendar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Google Client secret for accessing Calendar </t>
+  </si>
+  <si>
+    <t>Google location API end point</t>
+  </si>
+  <si>
+    <t>Open weather map end point</t>
   </si>
 </sst>
 </file>
@@ -563,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -627,6 +645,9 @@
       <c r="B3" t="s">
         <v>46</v>
       </c>
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -635,6 +656,9 @@
       <c r="B4" t="s">
         <v>48</v>
       </c>
+      <c r="C4" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -643,6 +667,9 @@
       <c r="B5" t="s">
         <v>50</v>
       </c>
+      <c r="C5" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -651,6 +678,9 @@
       <c r="B6" t="s">
         <v>52</v>
       </c>
+      <c r="C6" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -659,6 +689,9 @@
       <c r="B7" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="C7" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -666,6 +699,9 @@
       </c>
       <c r="B8" s="2" t="s">
         <v>55</v>
+      </c>
+      <c r="C8" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>